<commit_message>
worked in treaty. added merge countries, income, germplasm and fao
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\fao_sow\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F54DFD4-62CC-47D0-9279-1282C7B88770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883D0A63-020F-48F8-B813-DD4F455189D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
     <sheet name="plant_treaty" sheetId="5" r:id="rId2"/>
+    <sheet name="treaty_columns" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10957" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11137" uniqueCount="1577">
   <si>
     <t>value</t>
   </si>
@@ -4279,28 +4280,503 @@
     <t>plant_treaty_key_crop</t>
   </si>
   <si>
-    <t>ITPGRFA_MLS-Data-Store_2022_2_21.xlsx</t>
-  </si>
-  <si>
     <t>Genera - main,Taxa,Use - primary,Use - detailed,Use - alternates,Included in MLS Annex 1,Seed storage behaviour (Kew Seed Information Database)</t>
+  </si>
+  <si>
+    <t>countries_file</t>
+  </si>
+  <si>
+    <t>UNSD — Methodology.xlsx</t>
+  </si>
+  <si>
+    <t>ISO-alpha3 Code</t>
+  </si>
+  <si>
+    <t>countries_key_country</t>
+  </si>
+  <si>
+    <t>treaty_key_country_origin</t>
+  </si>
+  <si>
+    <t>treaty_key_country_recipient</t>
+  </si>
+  <si>
+    <t>ISO3</t>
+  </si>
+  <si>
+    <t>ISO3.1</t>
+  </si>
+  <si>
+    <t>countries_fields</t>
+  </si>
+  <si>
+    <t>Region Code,Region Name,Sub-region Code,Sub-region Name,Intermediate Region Code,Intermediate Region Name,Country or Area,ISO-alpha2 Code,ISO-alpha3 Code,Least Developed Countries (LDC),Land Locked Developing Countries (LLDC),Small Island Developing States (SIDS)</t>
+  </si>
+  <si>
+    <t>countries_sheet</t>
+  </si>
+  <si>
+    <t>UNSD — Methodology_filled</t>
+  </si>
+  <si>
+    <t>ITPGRFA_MLS-Data-Store_2022_2_22.xlsx</t>
+  </si>
+  <si>
+    <t>income_file</t>
+  </si>
+  <si>
+    <t>income_sheet</t>
+  </si>
+  <si>
+    <t>income_key</t>
+  </si>
+  <si>
+    <t>income_years</t>
+  </si>
+  <si>
+    <t>iso3</t>
+  </si>
+  <si>
+    <t>Country income category</t>
+  </si>
+  <si>
+    <t>Worldbank_historicalincomecategories_2022_2_22.xlsx</t>
+  </si>
+  <si>
+    <t>2010,2011,2012,2013,2014,2015,2016,2017,2018,2019,2020</t>
+  </si>
+  <si>
+    <t>treaty_year</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>germplasm_file</t>
+  </si>
+  <si>
+    <t>germplasm_sheet</t>
+  </si>
+  <si>
+    <t>germplasm_key</t>
+  </si>
+  <si>
+    <t>treaty_key_germplasm</t>
+  </si>
+  <si>
+    <t>Crop_cleaned</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>Germplasm_storage_type.xlsx</t>
+  </si>
+  <si>
+    <t>germplasm type</t>
+  </si>
+  <si>
+    <t>FoodBalanceSheets_E_All_Data.csv</t>
+  </si>
+  <si>
+    <t>fao_file</t>
+  </si>
+  <si>
+    <t>fao_years</t>
+  </si>
+  <si>
+    <t>Y2015,Y2016,Y2017,Y2018</t>
+  </si>
+  <si>
+    <t>fao_key_crop</t>
+  </si>
+  <si>
+    <t>fao_elements_col</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
+    <t>fao_encoding</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Provider country</t>
+  </si>
+  <si>
+    <t>Crop</t>
+  </si>
+  <si>
+    <t>Taxonomic name</t>
+  </si>
+  <si>
+    <t>Wild relative</t>
+  </si>
+  <si>
+    <t>Annex 1 or Article 15</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>Recipient country</t>
+  </si>
+  <si>
+    <t>Region Code_x</t>
+  </si>
+  <si>
+    <t>Region Name_x</t>
+  </si>
+  <si>
+    <t>Sub-region Code_x</t>
+  </si>
+  <si>
+    <t>Sub-region Name_x</t>
+  </si>
+  <si>
+    <t>Intermediate Region Code_x</t>
+  </si>
+  <si>
+    <t>Intermediate Region Name_x</t>
+  </si>
+  <si>
+    <t>Country or Area_x</t>
+  </si>
+  <si>
+    <t>ISO-alpha2 Code_x</t>
+  </si>
+  <si>
+    <t>ISO-alpha3 Code_x</t>
+  </si>
+  <si>
+    <t>Least Developed Countries (LDC)_x</t>
+  </si>
+  <si>
+    <t>Land Locked Developing Countries (LLDC)_x</t>
+  </si>
+  <si>
+    <t>Small Island Developing States (SIDS)_x</t>
+  </si>
+  <si>
+    <t>Region Code_y</t>
+  </si>
+  <si>
+    <t>Region Name_y</t>
+  </si>
+  <si>
+    <t>Sub-region Code_y</t>
+  </si>
+  <si>
+    <t>Sub-region Name_y</t>
+  </si>
+  <si>
+    <t>Intermediate Region Code_y</t>
+  </si>
+  <si>
+    <t>Intermediate Region Name_y</t>
+  </si>
+  <si>
+    <t>Country or Area_y</t>
+  </si>
+  <si>
+    <t>ISO-alpha2 Code_y</t>
+  </si>
+  <si>
+    <t>ISO-alpha3 Code_y</t>
+  </si>
+  <si>
+    <t>Least Developed Countries (LDC)_y</t>
+  </si>
+  <si>
+    <t>Land Locked Developing Countries (LLDC)_y</t>
+  </si>
+  <si>
+    <t>Small Island Developing States (SIDS)_y</t>
+  </si>
+  <si>
+    <t>iso3_x</t>
+  </si>
+  <si>
+    <t>value_x</t>
+  </si>
+  <si>
+    <t>iso3_y</t>
+  </si>
+  <si>
+    <t>value_y</t>
+  </si>
+  <si>
+    <t>Germplasm storage type</t>
+  </si>
+  <si>
+    <t>Domestic supply quantity</t>
+  </si>
+  <si>
+    <t>Export Quantity</t>
+  </si>
+  <si>
+    <t>Fat supply quantity (g/capita/day)</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>Food supply (kcal/capita/day)</t>
+  </si>
+  <si>
+    <t>Food supply quantity (kg/capita/yr)</t>
+  </si>
+  <si>
+    <t>Import Quantity</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>Other uses (non-food)</t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Protein supply quantity (g/capita/day)</t>
+  </si>
+  <si>
+    <t>Residuals</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Stock Variation</t>
+  </si>
+  <si>
+    <t>Tourist consumption</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>crop_cleaned</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>taxa</t>
+  </si>
+  <si>
+    <t>origin_iso3</t>
+  </si>
+  <si>
+    <t>origin_country</t>
+  </si>
+  <si>
+    <t>taxonomic_name</t>
+  </si>
+  <si>
+    <t>wild_relative</t>
+  </si>
+  <si>
+    <t>annex_1_or_article_15</t>
+  </si>
+  <si>
+    <t>crop_list_equivalent</t>
+  </si>
+  <si>
+    <t>recipient_iso3</t>
+  </si>
+  <si>
+    <t>recipient_country</t>
+  </si>
+  <si>
+    <t>genera_main</t>
+  </si>
+  <si>
+    <t>use_alternates</t>
+  </si>
+  <si>
+    <t>use_detailed</t>
+  </si>
+  <si>
+    <t>use_primary</t>
+  </si>
+  <si>
+    <t>plant</t>
+  </si>
+  <si>
+    <t>feed</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>losses</t>
+  </si>
+  <si>
+    <t>processing</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>residuals</t>
+  </si>
+  <si>
+    <t>seed</t>
+  </si>
+  <si>
+    <t>tourist_consumption</t>
+  </si>
+  <si>
+    <t>seed_storage</t>
+  </si>
+  <si>
+    <t>food_supply</t>
+  </si>
+  <si>
+    <t>other_uses</t>
+  </si>
+  <si>
+    <t>common_name_main</t>
+  </si>
+  <si>
+    <t>included_in_mls_annex_1</t>
+  </si>
+  <si>
+    <t>germplasm_storage_type</t>
+  </si>
+  <si>
+    <t>domestic_supply_quantity</t>
+  </si>
+  <si>
+    <t>origin_region_code</t>
+  </si>
+  <si>
+    <t>origin_region_name</t>
+  </si>
+  <si>
+    <t>origin_subregion_code</t>
+  </si>
+  <si>
+    <t>origin_subregion_name</t>
+  </si>
+  <si>
+    <t>origin_intermediate_region_code</t>
+  </si>
+  <si>
+    <t>origin_intermediate_region_name</t>
+  </si>
+  <si>
+    <t>origin_country_or_area</t>
+  </si>
+  <si>
+    <t>origin_iso_alpha2</t>
+  </si>
+  <si>
+    <t>origin_iso_alpha3</t>
+  </si>
+  <si>
+    <t>origin_least_developed_countries_ldc</t>
+  </si>
+  <si>
+    <t>origin_land_locked_developing_countries_lldc</t>
+  </si>
+  <si>
+    <t>origin_small_island_developing_states_sids</t>
+  </si>
+  <si>
+    <t>recipient_region_code</t>
+  </si>
+  <si>
+    <t>recipient_region_name</t>
+  </si>
+  <si>
+    <t>recipient_subregion_code</t>
+  </si>
+  <si>
+    <t>recipient_subregion_name</t>
+  </si>
+  <si>
+    <t>recipient_intermediate_region_code</t>
+  </si>
+  <si>
+    <t>recipient_intermediate_region_name</t>
+  </si>
+  <si>
+    <t>recipient_country_or_area</t>
+  </si>
+  <si>
+    <t>recipient_iso_alpha2</t>
+  </si>
+  <si>
+    <t>recipient_iso_alpha3</t>
+  </si>
+  <si>
+    <t>recipient_least_developed_countries_ldc</t>
+  </si>
+  <si>
+    <t>recipient_land_locked_developing_countries_lldc</t>
+  </si>
+  <si>
+    <t>recipient_small_island_developing_states_sids</t>
+  </si>
+  <si>
+    <t>origin_income_iso3</t>
+  </si>
+  <si>
+    <t>origin_income</t>
+  </si>
+  <si>
+    <t>recipient_income_iso3</t>
+  </si>
+  <si>
+    <t>recipient_income</t>
+  </si>
+  <si>
+    <t>export_quantity</t>
+  </si>
+  <si>
+    <t>fat_supply_quantity_g_capita_day</t>
+  </si>
+  <si>
+    <t>food_supply_quantity_kg_capita_yr</t>
+  </si>
+  <si>
+    <t>protein_supply_quantity_g_capita_day</t>
+  </si>
+  <si>
+    <t>import_quantity</t>
+  </si>
+  <si>
+    <t>stock_variation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4323,16 +4799,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4645,16 +5119,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -4678,7 +5152,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>1414</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4699,22 +5173,179 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1084</v>
+        <v>1419</v>
       </c>
       <c r="B6" t="s">
-        <v>1415</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>1413</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1426</v>
+      </c>
+    </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
+      <c r="A14" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4726,8 +5357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89DB26D6-2208-461C-8CAC-8D8F44D98323}">
   <dimension ref="A1:BJ356"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38276,4 +38907,583 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C2A8A4-DA1A-428D-90DC-2778CD784C14}">
+  <dimension ref="A1:B70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>1469</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added nagoya and cleaned columns names
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\fao_sow\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883D0A63-020F-48F8-B813-DD4F455189D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405CE1CB-698A-4611-ADEA-8590726FCDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11137" uniqueCount="1577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11164" uniqueCount="1602">
   <si>
     <t>value</t>
   </si>
@@ -4649,9 +4649,6 @@
     <t>seed_storage</t>
   </si>
   <si>
-    <t>food_supply</t>
-  </si>
-  <si>
     <t>other_uses</t>
   </si>
   <si>
@@ -4767,6 +4764,84 @@
   </si>
   <si>
     <t>stock_variation</t>
+  </si>
+  <si>
+    <t>drop</t>
+  </si>
+  <si>
+    <t>food_supply_kcal_capita_day</t>
+  </si>
+  <si>
+    <t>nagoya_file</t>
+  </si>
+  <si>
+    <t>nagoya_sheet</t>
+  </si>
+  <si>
+    <t>nagoya_key</t>
+  </si>
+  <si>
+    <t>Nagoya_cleaned</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Nagoya_Country Ratification_02.08.22_cleaned.xlsx</t>
+  </si>
+  <si>
+    <t>treaty_name_country_origin</t>
+  </si>
+  <si>
+    <t>treaty_name_country_recipient</t>
+  </si>
+  <si>
+    <t>Country_x</t>
+  </si>
+  <si>
+    <t>Ratification_1_x</t>
+  </si>
+  <si>
+    <t>Party_cleaned_x</t>
+  </si>
+  <si>
+    <t>Party_year_cleaned_x</t>
+  </si>
+  <si>
+    <t>Country_y</t>
+  </si>
+  <si>
+    <t>Ratification_1_y</t>
+  </si>
+  <si>
+    <t>Party_cleaned_y</t>
+  </si>
+  <si>
+    <t>Party_year_cleaned_y</t>
+  </si>
+  <si>
+    <t>origin_nagoya_ratification_1</t>
+  </si>
+  <si>
+    <t>origin_nagoya_party_cleaned</t>
+  </si>
+  <si>
+    <t>origin_nagoya_party_year_cleaned</t>
+  </si>
+  <si>
+    <t>origin_nagoya_country</t>
+  </si>
+  <si>
+    <t>recipient_nagoya_country</t>
+  </si>
+  <si>
+    <t>recipient_nagoya_ratification_1</t>
+  </si>
+  <si>
+    <t>recipient_nagoya_party_cleaned</t>
+  </si>
+  <si>
+    <t>recipient_nagoya_party_year_cleaned</t>
   </si>
 </sst>
 </file>
@@ -5119,10 +5194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5189,162 +5264,202 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1441</v>
+        <v>1584</v>
       </c>
       <c r="B8" t="s">
-        <v>1442</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1436</v>
+        <v>1585</v>
       </c>
       <c r="B9" t="s">
-        <v>1437</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1084</v>
+        <v>1441</v>
       </c>
       <c r="B10" t="s">
-        <v>1414</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1413</v>
+        <v>1436</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1415</v>
+        <v>1084</v>
       </c>
       <c r="B12" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1425</v>
+        <v>1413</v>
       </c>
       <c r="B13" t="s">
-        <v>1426</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1423</v>
+        <v>1415</v>
       </c>
       <c r="B14" t="s">
-        <v>1424</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1418</v>
+        <v>1425</v>
       </c>
       <c r="B15" t="s">
-        <v>1417</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="B16" t="s">
-        <v>1434</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1429</v>
+        <v>1418</v>
       </c>
       <c r="B17" t="s">
-        <v>1433</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="B18" t="s">
-        <v>1432</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1431</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1435</v>
+        <v>1429</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1433</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1438</v>
+        <v>1430</v>
       </c>
       <c r="B20" t="s">
-        <v>1444</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1445</v>
+        <v>1431</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1435</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="B22" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1447</v>
+        <v>1439</v>
       </c>
       <c r="B23" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1448</v>
+        <v>1440</v>
       </c>
       <c r="B24" t="s">
-        <v>1449</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="B25" t="s">
-        <v>1452</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="B26" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>1454</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1582</v>
       </c>
     </row>
   </sheetData>
@@ -38911,576 +39026,874 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C2A8A4-DA1A-428D-90DC-2778CD784C14}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1508</v>
       </c>
       <c r="B1" t="s">
         <v>1509</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1455</v>
       </c>
       <c r="B2" t="s">
         <v>1510</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1421</v>
       </c>
       <c r="B3" t="s">
         <v>1515</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1456</v>
       </c>
       <c r="B4" t="s">
         <v>1516</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1457</v>
       </c>
       <c r="B5" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1442</v>
       </c>
       <c r="B6" t="s">
         <v>1511</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1458</v>
       </c>
       <c r="B7" t="s">
         <v>1517</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1459</v>
       </c>
       <c r="B8" t="s">
         <v>1518</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1460</v>
       </c>
       <c r="B9" t="s">
         <v>1519</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1411</v>
       </c>
       <c r="B10" t="s">
         <v>1520</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1437</v>
       </c>
       <c r="B11" t="s">
         <v>1512</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1461</v>
       </c>
       <c r="B12" t="s">
         <v>1513</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1422</v>
       </c>
       <c r="B13" t="s">
         <v>1521</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1462</v>
       </c>
       <c r="B14" t="s">
         <v>1522</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>1523</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>1514</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>1524</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1110</v>
       </c>
       <c r="B18" t="s">
         <v>1536</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1538</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>1525</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>1526</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1099</v>
       </c>
       <c r="B22" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1539</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1463</v>
       </c>
       <c r="B23" t="s">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1542</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1464</v>
       </c>
       <c r="B24" t="s">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1543</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1465</v>
       </c>
       <c r="B25" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1544</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1466</v>
       </c>
       <c r="B26" t="s">
-        <v>1546</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1545</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1467</v>
       </c>
       <c r="B27" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1546</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1468</v>
       </c>
       <c r="B28" t="s">
-        <v>1548</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1547</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1469</v>
       </c>
       <c r="B29" t="s">
-        <v>1549</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1548</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1470</v>
       </c>
       <c r="B30" t="s">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1549</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1471</v>
       </c>
       <c r="B31" t="s">
-        <v>1551</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1550</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1472</v>
       </c>
       <c r="B32" t="s">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1551</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1473</v>
       </c>
       <c r="B33" t="s">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1552</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1474</v>
       </c>
       <c r="B34" t="s">
-        <v>1554</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1553</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1475</v>
       </c>
       <c r="B35" t="s">
-        <v>1555</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1554</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1476</v>
       </c>
       <c r="B36" t="s">
-        <v>1556</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1555</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1477</v>
       </c>
       <c r="B37" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1556</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1478</v>
       </c>
       <c r="B38" t="s">
-        <v>1558</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1557</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1479</v>
       </c>
       <c r="B39" t="s">
-        <v>1559</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1558</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>1480</v>
       </c>
       <c r="B40" t="s">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1559</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>1481</v>
       </c>
       <c r="B41" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1560</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1482</v>
       </c>
       <c r="B42" t="s">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1561</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>1483</v>
       </c>
       <c r="B43" t="s">
-        <v>1563</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1562</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1484</v>
       </c>
       <c r="B44" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1563</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1485</v>
       </c>
       <c r="B45" t="s">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1564</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1486</v>
       </c>
       <c r="B46" t="s">
-        <v>1566</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1565</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1487</v>
       </c>
       <c r="B47" t="s">
-        <v>1567</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1566</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1488</v>
       </c>
       <c r="B48" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1567</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>1489</v>
       </c>
       <c r="B49" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1568</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1490</v>
       </c>
       <c r="B50" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1569</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>1443</v>
       </c>
       <c r="B51" t="s">
         <v>1527</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>1491</v>
       </c>
       <c r="B52" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1540</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1453</v>
       </c>
       <c r="B53" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>1492</v>
       </c>
       <c r="B54" t="s">
-        <v>1542</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1541</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>1493</v>
       </c>
       <c r="B55" t="s">
-        <v>1571</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1570</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>1494</v>
       </c>
       <c r="B56" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1571</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>1495</v>
       </c>
       <c r="B57" t="s">
         <v>1528</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>22</v>
       </c>
       <c r="B58" t="s">
         <v>1529</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>1496</v>
       </c>
       <c r="B59" t="s">
-        <v>1537</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1577</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>1497</v>
       </c>
       <c r="B60" t="s">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1572</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>1498</v>
       </c>
       <c r="B61" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1574</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>1499</v>
       </c>
       <c r="B62" t="s">
         <v>1530</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>1500</v>
       </c>
       <c r="B63" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1537</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>1501</v>
       </c>
       <c r="B64" t="s">
         <v>1531</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>1502</v>
       </c>
       <c r="B65" t="s">
         <v>1532</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1503</v>
       </c>
       <c r="B66" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1573</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>1504</v>
       </c>
       <c r="B67" t="s">
         <v>1533</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>1505</v>
       </c>
       <c r="B68" t="s">
         <v>1534</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>1506</v>
       </c>
       <c r="B69" t="s">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1575</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>1507</v>
       </c>
       <c r="B70" t="s">
         <v>1535</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added other fao files and members of treaty
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\fao_sow\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405CE1CB-698A-4611-ADEA-8590726FCDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A732807-D24A-4BD4-B971-73E9A864E8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11164" uniqueCount="1602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11224" uniqueCount="1654">
   <si>
     <t>value</t>
   </si>
@@ -4376,12 +4376,6 @@
     <t>germplasm type</t>
   </si>
   <si>
-    <t>FoodBalanceSheets_E_All_Data.csv</t>
-  </si>
-  <si>
-    <t>fao_file</t>
-  </si>
-  <si>
     <t>fao_years</t>
   </si>
   <si>
@@ -4842,6 +4836,168 @@
   </si>
   <si>
     <t>recipient_nagoya_party_year_cleaned</t>
+  </si>
+  <si>
+    <t>origin_nagoya_transfer</t>
+  </si>
+  <si>
+    <t>recipient_nagoya_transfer</t>
+  </si>
+  <si>
+    <t>nagoya_key_year</t>
+  </si>
+  <si>
+    <t>Party_year_cleaned</t>
+  </si>
+  <si>
+    <t>member_file</t>
+  </si>
+  <si>
+    <t>member_sheet</t>
+  </si>
+  <si>
+    <t>member_key</t>
+  </si>
+  <si>
+    <t>member_key_year</t>
+  </si>
+  <si>
+    <t>ITPGRFA_Membership_List_20220215_cleaned.xlsx</t>
+  </si>
+  <si>
+    <t>Membership_List_20220215</t>
+  </si>
+  <si>
+    <t>Entry into Force_cleaned</t>
+  </si>
+  <si>
+    <t>FoodBalanceSheets_E_All_Data.csv,Production_Crops_E_All_Data.csv,Value_of_Production_E_All_Data.csv</t>
+  </si>
+  <si>
+    <t>fao_files</t>
+  </si>
+  <si>
+    <t>crop_y</t>
+  </si>
+  <si>
+    <t>Area harvested</t>
+  </si>
+  <si>
+    <t>Production_y</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>Gross Production Value (constant 2014-2016 thousand I$)</t>
+  </si>
+  <si>
+    <t>Gross Production Value (constant 2014-2016 thousand SLC)</t>
+  </si>
+  <si>
+    <t>Gross Production Value (constant 2014-2016 thousand US$)</t>
+  </si>
+  <si>
+    <t>Gross Production Value (current thousand SLC)</t>
+  </si>
+  <si>
+    <t>Gross Production Value (current thousand US$)</t>
+  </si>
+  <si>
+    <t>crop_fao</t>
+  </si>
+  <si>
+    <t>fao_area_harvested</t>
+  </si>
+  <si>
+    <t>fao_yield</t>
+  </si>
+  <si>
+    <t>fao_production</t>
+  </si>
+  <si>
+    <t>crop_fao2</t>
+  </si>
+  <si>
+    <t>fao_gpv_constant_2014_2016_thousand_i</t>
+  </si>
+  <si>
+    <t>fao_gpv_constant_2014_2016_thousand_us</t>
+  </si>
+  <si>
+    <t>fao_gpv_constant_2014_2016_thousand_slc</t>
+  </si>
+  <si>
+    <t>fao_gpv_current_slc</t>
+  </si>
+  <si>
+    <t>fao_gpv_current_us</t>
+  </si>
+  <si>
+    <t>Contracting Party_x</t>
+  </si>
+  <si>
+    <t>Contracting Party_cleaned_x</t>
+  </si>
+  <si>
+    <t>Entry into Force_x</t>
+  </si>
+  <si>
+    <t>Entry into Force_cleaned_x</t>
+  </si>
+  <si>
+    <t>ISO3_y</t>
+  </si>
+  <si>
+    <t>Contracting Party_y</t>
+  </si>
+  <si>
+    <t>Contracting Party_cleaned_y</t>
+  </si>
+  <si>
+    <t>Entry into Force_y</t>
+  </si>
+  <si>
+    <t>Entry into Force_cleaned_y</t>
+  </si>
+  <si>
+    <t>origin_member_treaty_transfer</t>
+  </si>
+  <si>
+    <t>recipient_member_treaty_transfer</t>
+  </si>
+  <si>
+    <t>origin_member_treaty_country</t>
+  </si>
+  <si>
+    <t>origin_member_treaty_contracting_party</t>
+  </si>
+  <si>
+    <t>origin_member_treaty_contracting_party_cleaned</t>
+  </si>
+  <si>
+    <t>origin_member_treaty_entry_into_force_cleaned</t>
+  </si>
+  <si>
+    <t>origin_member_treaty_entry_into_force</t>
+  </si>
+  <si>
+    <t>recipient_member_treaty_country</t>
+  </si>
+  <si>
+    <t>recipient_member_treaty_iso3</t>
+  </si>
+  <si>
+    <t>recipient_member_treaty_contracting party</t>
+  </si>
+  <si>
+    <t>recipient_member_treaty_contracting party_cleaned</t>
+  </si>
+  <si>
+    <t>recipient_member_treaty_entry into force</t>
+  </si>
+  <si>
+    <t>recipient_member_treaty_entry into force_cleaned</t>
   </si>
 </sst>
 </file>
@@ -5194,10 +5350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5264,18 +5420,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="B8" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="B9" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5400,39 +5556,39 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1447</v>
+        <v>1612</v>
       </c>
       <c r="B25" t="s">
-        <v>1446</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="B26" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="B27" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="B28" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
@@ -5440,26 +5596,66 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="B30" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B31" t="s">
         <v>1579</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1581</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B32" t="s">
         <v>1580</v>
       </c>
-      <c r="B32" t="s">
-        <v>1582</v>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>1607</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1610</v>
       </c>
     </row>
   </sheetData>
@@ -39026,10 +39222,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C2A8A4-DA1A-428D-90DC-2778CD784C14}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39040,21 +39236,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="B1" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="C1" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="B2" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -39065,7 +39261,7 @@
         <v>1421</v>
       </c>
       <c r="B3" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -39073,10 +39269,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="B4" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -39084,10 +39280,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="B5" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -39098,7 +39294,7 @@
         <v>1442</v>
       </c>
       <c r="B6" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -39106,10 +39302,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="B7" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -39117,10 +39313,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="B8" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -39128,10 +39324,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="B9" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -39142,7 +39338,7 @@
         <v>1411</v>
       </c>
       <c r="B10" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -39153,7 +39349,7 @@
         <v>1437</v>
       </c>
       <c r="B11" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -39161,10 +39357,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="B12" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -39175,7 +39371,7 @@
         <v>1422</v>
       </c>
       <c r="B13" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -39183,10 +39379,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="B14" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -39197,7 +39393,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -39208,7 +39404,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -39219,7 +39415,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -39230,7 +39426,7 @@
         <v>1110</v>
       </c>
       <c r="B18" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -39241,7 +39437,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -39252,7 +39448,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -39263,7 +39459,7 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -39274,7 +39470,7 @@
         <v>1099</v>
       </c>
       <c r="B22" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -39282,10 +39478,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="B23" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -39293,10 +39489,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="B24" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -39304,10 +39500,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="B25" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -39315,10 +39511,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="B26" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -39326,10 +39522,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="B27" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -39337,10 +39533,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="B28" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -39348,10 +39544,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="B29" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -39359,10 +39555,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="B30" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -39370,10 +39566,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="B31" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -39381,10 +39577,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="B32" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -39392,10 +39588,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="B33" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -39403,10 +39599,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="B34" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -39414,10 +39610,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="B35" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -39425,10 +39621,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="B36" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -39436,10 +39632,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="B37" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -39447,10 +39643,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="B38" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -39458,10 +39654,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="B39" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -39469,10 +39665,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="B40" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -39480,10 +39676,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="B41" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -39491,10 +39687,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="B42" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -39502,10 +39698,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="B43" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -39513,10 +39709,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="B44" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -39524,10 +39720,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="B45" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -39535,10 +39731,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="B46" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -39546,10 +39742,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="B47" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -39557,10 +39753,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="B48" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -39568,10 +39764,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="B49" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -39579,10 +39775,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="B50" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -39593,7 +39789,7 @@
         <v>1443</v>
       </c>
       <c r="B51" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -39601,10 +39797,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="B52" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -39612,10 +39808,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="B53" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -39623,10 +39819,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="B54" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -39634,10 +39830,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="B55" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -39645,10 +39841,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="B56" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -39656,10 +39852,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="B57" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -39670,7 +39866,7 @@
         <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -39678,10 +39874,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="B59" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -39689,10 +39885,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="B60" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -39700,10 +39896,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="B61" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -39711,10 +39907,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="B62" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -39722,21 +39918,21 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="B63" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="B64" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -39744,10 +39940,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="B65" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -39755,10 +39951,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="B66" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -39766,10 +39962,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="B67" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -39777,10 +39973,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="B68" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -39788,10 +39984,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="B69" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -39799,10 +39995,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="B70" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -39810,10 +40006,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1586</v>
+        <v>1613</v>
       </c>
       <c r="B71" t="s">
-        <v>1597</v>
+        <v>1622</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -39821,10 +40017,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1587</v>
+        <v>1614</v>
       </c>
       <c r="B72" t="s">
-        <v>1594</v>
+        <v>1623</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -39832,10 +40028,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1588</v>
+        <v>1615</v>
       </c>
       <c r="B73" t="s">
-        <v>1595</v>
+        <v>1625</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -39843,21 +40039,21 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1589</v>
+        <v>1616</v>
       </c>
       <c r="B74" t="s">
-        <v>1596</v>
+        <v>1624</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>1590</v>
+        <v>1451</v>
       </c>
       <c r="B75" t="s">
-        <v>1598</v>
+        <v>1626</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -39865,34 +40061,309 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>1591</v>
+        <v>1617</v>
       </c>
       <c r="B76" t="s">
-        <v>1599</v>
+        <v>1627</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>1592</v>
+        <v>1618</v>
       </c>
       <c r="B77" t="s">
-        <v>1600</v>
+        <v>1629</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1630</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B83" t="s">
         <v>1593</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>1601</v>
       </c>
-      <c r="C78">
+      <c r="B90" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1644</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>1635</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1646</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1648</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1649</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>1637</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1650</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1652</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1653</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C103">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed columns names in conf file
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\fao_sow\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A732807-D24A-4BD4-B971-73E9A864E8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301003C4-96B6-4DA0-9C66-7A396030940E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11224" uniqueCount="1654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11328" uniqueCount="1665">
   <si>
     <t>value</t>
   </si>
@@ -4998,6 +4998,39 @@
   </si>
   <si>
     <t>recipient_member_treaty_entry into force_cleaned</t>
+  </si>
+  <si>
+    <t>new_1</t>
+  </si>
+  <si>
+    <t>drop_1</t>
+  </si>
+  <si>
+    <t>crop_original</t>
+  </si>
+  <si>
+    <t>Number_of_samples</t>
+  </si>
+  <si>
+    <t>seed_storage_behavior</t>
+  </si>
+  <si>
+    <t>included_in_mls_annex1</t>
+  </si>
+  <si>
+    <t>production_area_harvested</t>
+  </si>
+  <si>
+    <t>production_quantity</t>
+  </si>
+  <si>
+    <t>production_value_cnst_2014-16_us</t>
+  </si>
+  <si>
+    <t>origin_member_nagoya_transfer</t>
+  </si>
+  <si>
+    <t>recipient_member_nagoya_transfer</t>
   </si>
 </sst>
 </file>
@@ -39222,10 +39255,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C2A8A4-DA1A-428D-90DC-2778CD784C14}">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39234,1136 +39267,1754 @@
     <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1506</v>
       </c>
       <c r="B1" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C1" t="s">
         <v>1507</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="E1" t="s">
         <v>1574</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1453</v>
       </c>
       <c r="B2" t="s">
         <v>1508</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1421</v>
       </c>
       <c r="B3" t="s">
         <v>1513</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1454</v>
       </c>
       <c r="B4" t="s">
         <v>1514</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>1514</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1455</v>
       </c>
       <c r="B5" t="s">
         <v>1451</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>1656</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1442</v>
       </c>
       <c r="B6" t="s">
         <v>1509</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>1509</v>
+      </c>
+      <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1456</v>
       </c>
       <c r="B7" t="s">
         <v>1515</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1457</v>
       </c>
       <c r="B8" t="s">
         <v>1516</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1458</v>
       </c>
       <c r="B9" t="s">
         <v>1517</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>1517</v>
+      </c>
+      <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1411</v>
       </c>
       <c r="B10" t="s">
         <v>1518</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>1518</v>
+      </c>
+      <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1437</v>
       </c>
       <c r="B11" t="s">
         <v>1510</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1459</v>
       </c>
       <c r="B12" t="s">
         <v>1511</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1422</v>
       </c>
       <c r="B13" t="s">
         <v>1519</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1460</v>
       </c>
       <c r="B14" t="s">
         <v>1520</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>1521</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>1512</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>1522</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1110</v>
       </c>
       <c r="B18" t="s">
         <v>1534</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>1536</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>1523</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>1523</v>
+      </c>
+      <c r="D20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>1524</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1099</v>
       </c>
       <c r="B22" t="s">
         <v>1537</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1461</v>
       </c>
       <c r="B23" t="s">
         <v>1540</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1462</v>
       </c>
       <c r="B24" t="s">
         <v>1541</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1463</v>
       </c>
       <c r="B25" t="s">
         <v>1542</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1464</v>
       </c>
       <c r="B26" t="s">
         <v>1543</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1465</v>
       </c>
       <c r="B27" t="s">
         <v>1544</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1466</v>
       </c>
       <c r="B28" t="s">
         <v>1545</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1467</v>
       </c>
       <c r="B29" t="s">
         <v>1546</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1468</v>
       </c>
       <c r="B30" t="s">
         <v>1547</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>1547</v>
+      </c>
+      <c r="D30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1469</v>
       </c>
       <c r="B31" t="s">
         <v>1548</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1470</v>
       </c>
       <c r="B32" t="s">
         <v>1549</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>1549</v>
+      </c>
+      <c r="D32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1471</v>
       </c>
       <c r="B33" t="s">
         <v>1550</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1472</v>
       </c>
       <c r="B34" t="s">
         <v>1551</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1473</v>
       </c>
       <c r="B35" t="s">
         <v>1552</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="s">
+        <v>1552</v>
+      </c>
+      <c r="D35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1474</v>
       </c>
       <c r="B36" t="s">
         <v>1553</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1475</v>
       </c>
       <c r="B37" t="s">
         <v>1554</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1476</v>
       </c>
       <c r="B38" t="s">
         <v>1555</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1477</v>
       </c>
       <c r="B39" t="s">
         <v>1556</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="s">
+        <v>1556</v>
+      </c>
+      <c r="D39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>1478</v>
       </c>
       <c r="B40" t="s">
         <v>1557</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="s">
+        <v>1557</v>
+      </c>
+      <c r="D40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>1479</v>
       </c>
       <c r="B41" t="s">
         <v>1558</v>
       </c>
-      <c r="C41">
+      <c r="C41" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1480</v>
       </c>
       <c r="B42" t="s">
         <v>1559</v>
       </c>
-      <c r="C42">
+      <c r="C42" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>1481</v>
       </c>
       <c r="B43" t="s">
         <v>1560</v>
       </c>
-      <c r="C43">
+      <c r="C43" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1482</v>
       </c>
       <c r="B44" t="s">
         <v>1561</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1483</v>
       </c>
       <c r="B45" t="s">
         <v>1562</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1484</v>
       </c>
       <c r="B46" t="s">
         <v>1563</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1485</v>
       </c>
       <c r="B47" t="s">
         <v>1564</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1486</v>
       </c>
       <c r="B48" t="s">
         <v>1565</v>
       </c>
-      <c r="C48">
+      <c r="C48" t="s">
+        <v>1565</v>
+      </c>
+      <c r="D48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>1487</v>
       </c>
       <c r="B49" t="s">
         <v>1566</v>
       </c>
-      <c r="C49">
+      <c r="C49" t="s">
+        <v>1566</v>
+      </c>
+      <c r="D49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1488</v>
       </c>
       <c r="B50" t="s">
         <v>1567</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="s">
+        <v>1567</v>
+      </c>
+      <c r="D50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>1443</v>
       </c>
       <c r="B51" t="s">
         <v>1525</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>1489</v>
       </c>
       <c r="B52" t="s">
         <v>1538</v>
       </c>
-      <c r="C52">
+      <c r="C52" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1451</v>
       </c>
       <c r="B53" t="s">
         <v>1451</v>
       </c>
-      <c r="C53">
+      <c r="C53" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>1490</v>
       </c>
       <c r="B54" t="s">
         <v>1539</v>
       </c>
-      <c r="C54">
+      <c r="C54" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>1491</v>
       </c>
       <c r="B55" t="s">
         <v>1568</v>
       </c>
-      <c r="C55">
+      <c r="C55" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>1492</v>
       </c>
       <c r="B56" t="s">
         <v>1569</v>
       </c>
-      <c r="C56">
+      <c r="C56" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>1493</v>
       </c>
       <c r="B57" t="s">
         <v>1526</v>
       </c>
-      <c r="C57">
+      <c r="C57" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>22</v>
       </c>
       <c r="B58" t="s">
         <v>1527</v>
       </c>
-      <c r="C58">
+      <c r="C58" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>1494</v>
       </c>
       <c r="B59" t="s">
         <v>1575</v>
       </c>
-      <c r="C59">
+      <c r="C59" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>1495</v>
       </c>
       <c r="B60" t="s">
         <v>1570</v>
       </c>
-      <c r="C60">
+      <c r="C60" t="s">
+        <v>1570</v>
+      </c>
+      <c r="D60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>1496</v>
       </c>
       <c r="B61" t="s">
         <v>1572</v>
       </c>
-      <c r="C61">
+      <c r="C61" t="s">
+        <v>1572</v>
+      </c>
+      <c r="D61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>1497</v>
       </c>
       <c r="B62" t="s">
         <v>1528</v>
       </c>
-      <c r="C62">
+      <c r="C62" t="s">
+        <v>1528</v>
+      </c>
+      <c r="D62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>1498</v>
       </c>
       <c r="B63" t="s">
         <v>1535</v>
       </c>
-      <c r="C63">
+      <c r="C63" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>1499</v>
       </c>
       <c r="B64" t="s">
         <v>1529</v>
       </c>
-      <c r="C64">
+      <c r="C64" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>1500</v>
       </c>
       <c r="B65" t="s">
         <v>1530</v>
       </c>
-      <c r="C65">
+      <c r="C65" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1501</v>
       </c>
       <c r="B66" t="s">
         <v>1571</v>
       </c>
-      <c r="C66">
+      <c r="C66" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>1502</v>
       </c>
       <c r="B67" t="s">
         <v>1531</v>
       </c>
-      <c r="C67">
+      <c r="C67" t="s">
+        <v>1531</v>
+      </c>
+      <c r="D67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>1503</v>
       </c>
       <c r="B68" t="s">
         <v>1532</v>
       </c>
-      <c r="C68">
+      <c r="C68" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>1504</v>
       </c>
       <c r="B69" t="s">
         <v>1573</v>
       </c>
-      <c r="C69">
+      <c r="C69" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>1505</v>
       </c>
       <c r="B70" t="s">
         <v>1533</v>
       </c>
-      <c r="C70">
+      <c r="C70" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>1613</v>
       </c>
       <c r="B71" t="s">
         <v>1622</v>
       </c>
-      <c r="C71">
+      <c r="C71" t="s">
+        <v>1622</v>
+      </c>
+      <c r="D71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>1614</v>
       </c>
       <c r="B72" t="s">
         <v>1623</v>
       </c>
-      <c r="C72">
+      <c r="C72" t="s">
+        <v>1660</v>
+      </c>
+      <c r="D72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>1615</v>
       </c>
       <c r="B73" t="s">
         <v>1625</v>
       </c>
-      <c r="C73">
+      <c r="C73" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>1616</v>
       </c>
       <c r="B74" t="s">
         <v>1624</v>
       </c>
-      <c r="C74">
+      <c r="C74" t="s">
+        <v>1624</v>
+      </c>
+      <c r="D74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>1451</v>
       </c>
       <c r="B75" t="s">
         <v>1626</v>
       </c>
-      <c r="C75">
+      <c r="C75" t="s">
+        <v>1626</v>
+      </c>
+      <c r="D75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>1617</v>
       </c>
       <c r="B76" t="s">
         <v>1627</v>
       </c>
-      <c r="C76">
+      <c r="C76" t="s">
+        <v>1627</v>
+      </c>
+      <c r="D76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>1618</v>
       </c>
       <c r="B77" t="s">
         <v>1629</v>
       </c>
-      <c r="C77">
+      <c r="C77" t="s">
+        <v>1629</v>
+      </c>
+      <c r="D77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>1619</v>
       </c>
       <c r="B78" t="s">
         <v>1628</v>
       </c>
-      <c r="C78">
+      <c r="C78" t="s">
+        <v>1662</v>
+      </c>
+      <c r="D78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>1620</v>
       </c>
       <c r="B79" t="s">
         <v>1630</v>
       </c>
-      <c r="C79">
+      <c r="C79" t="s">
+        <v>1630</v>
+      </c>
+      <c r="D79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>1621</v>
       </c>
       <c r="B80" t="s">
         <v>1631</v>
       </c>
-      <c r="C80">
+      <c r="C80" t="s">
+        <v>1631</v>
+      </c>
+      <c r="D80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>1584</v>
       </c>
       <c r="B81" t="s">
         <v>1595</v>
       </c>
-      <c r="C81">
+      <c r="C81" t="s">
+        <v>1595</v>
+      </c>
+      <c r="D81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>1585</v>
       </c>
       <c r="B82" t="s">
         <v>1592</v>
       </c>
-      <c r="C82">
+      <c r="C82" t="s">
+        <v>1592</v>
+      </c>
+      <c r="D82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>1586</v>
       </c>
       <c r="B83" t="s">
         <v>1593</v>
       </c>
-      <c r="C83">
+      <c r="C83" t="s">
+        <v>1593</v>
+      </c>
+      <c r="D83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>1587</v>
       </c>
       <c r="B84" t="s">
         <v>1594</v>
       </c>
-      <c r="C84">
+      <c r="C84" t="s">
+        <v>1594</v>
+      </c>
+      <c r="D84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>1588</v>
       </c>
       <c r="B85" t="s">
         <v>1596</v>
       </c>
-      <c r="C85">
+      <c r="C85" t="s">
+        <v>1596</v>
+      </c>
+      <c r="D85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>1589</v>
       </c>
       <c r="B86" t="s">
         <v>1597</v>
       </c>
-      <c r="C86">
+      <c r="C86" t="s">
+        <v>1597</v>
+      </c>
+      <c r="D86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>1590</v>
       </c>
       <c r="B87" t="s">
         <v>1598</v>
       </c>
-      <c r="C87">
+      <c r="C87" t="s">
+        <v>1598</v>
+      </c>
+      <c r="D87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>1591</v>
       </c>
       <c r="B88" t="s">
         <v>1599</v>
       </c>
-      <c r="C88">
+      <c r="C88" t="s">
+        <v>1599</v>
+      </c>
+      <c r="D88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>1600</v>
       </c>
       <c r="B89" t="s">
         <v>1600</v>
       </c>
-      <c r="C89">
+      <c r="C89" t="s">
+        <v>1663</v>
+      </c>
+      <c r="D89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>1601</v>
       </c>
       <c r="B90" t="s">
         <v>1601</v>
       </c>
-      <c r="C90">
+      <c r="C90" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>1584</v>
       </c>
       <c r="B91" t="s">
         <v>1643</v>
       </c>
-      <c r="C91">
+      <c r="C91" t="s">
+        <v>1643</v>
+      </c>
+      <c r="D91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>1632</v>
       </c>
       <c r="B92" t="s">
         <v>1644</v>
       </c>
-      <c r="C92">
+      <c r="C92" t="s">
+        <v>1644</v>
+      </c>
+      <c r="D92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>1633</v>
       </c>
       <c r="B93" t="s">
         <v>1645</v>
       </c>
-      <c r="C93">
+      <c r="C93" t="s">
+        <v>1645</v>
+      </c>
+      <c r="D93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>1634</v>
       </c>
       <c r="B94" t="s">
         <v>1647</v>
       </c>
-      <c r="C94">
+      <c r="C94" t="s">
+        <v>1647</v>
+      </c>
+      <c r="D94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>1635</v>
       </c>
       <c r="B95" t="s">
         <v>1646</v>
       </c>
-      <c r="C95">
+      <c r="C95" t="s">
+        <v>1646</v>
+      </c>
+      <c r="D95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>1588</v>
       </c>
       <c r="B96" t="s">
         <v>1648</v>
       </c>
-      <c r="C96">
+      <c r="C96" t="s">
+        <v>1648</v>
+      </c>
+      <c r="D96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>1636</v>
       </c>
       <c r="B97" t="s">
         <v>1649</v>
       </c>
-      <c r="C97">
+      <c r="C97" t="s">
+        <v>1649</v>
+      </c>
+      <c r="D97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>1637</v>
       </c>
       <c r="B98" t="s">
         <v>1650</v>
       </c>
-      <c r="C98">
+      <c r="C98" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>1638</v>
       </c>
       <c r="B99" t="s">
         <v>1651</v>
       </c>
-      <c r="C99">
+      <c r="C99" t="s">
+        <v>1651</v>
+      </c>
+      <c r="D99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>1639</v>
       </c>
       <c r="B100" t="s">
         <v>1652</v>
       </c>
-      <c r="C100">
+      <c r="C100" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>1640</v>
       </c>
       <c r="B101" t="s">
         <v>1653</v>
       </c>
-      <c r="C101">
+      <c r="C101" t="s">
+        <v>1653</v>
+      </c>
+      <c r="D101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>1641</v>
       </c>
       <c r="B102" t="s">
         <v>1641</v>
       </c>
-      <c r="C102">
+      <c r="C102" t="s">
+        <v>1641</v>
+      </c>
+      <c r="D102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>1642</v>
       </c>
       <c r="B103" t="s">
         <v>1642</v>
       </c>
-      <c r="C103">
+      <c r="C103" t="s">
+        <v>1642</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added fao views code
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\fao_sow\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301003C4-96B6-4DA0-9C66-7A396030940E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153CD56C-CB3E-4588-A799-C310C9C9794F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
     <sheet name="plant_treaty" sheetId="5" r:id="rId2"/>
     <sheet name="treaty_columns" sheetId="6" r:id="rId3"/>
+    <sheet name="fao_views_columns" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11328" uniqueCount="1665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11651" uniqueCount="1734">
   <si>
     <t>value</t>
   </si>
@@ -4781,9 +4782,6 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Nagoya_Country Ratification_02.08.22_cleaned.xlsx</t>
-  </si>
-  <si>
     <t>treaty_name_country_origin</t>
   </si>
   <si>
@@ -5031,6 +5029,216 @@
   </si>
   <si>
     <t>recipient_member_nagoya_transfer</t>
+  </si>
+  <si>
+    <t>fao_views_encoding</t>
+  </si>
+  <si>
+    <t>fao_views_file</t>
+  </si>
+  <si>
+    <t>fao_views_sheet</t>
+  </si>
+  <si>
+    <t>fao_views_key_country_origin</t>
+  </si>
+  <si>
+    <t>fao_views_key_germplasm</t>
+  </si>
+  <si>
+    <t>fao_views_year</t>
+  </si>
+  <si>
+    <t>FAO_WIEWS_Fulldataset</t>
+  </si>
+  <si>
+    <t>Crop_List_equivalent</t>
+  </si>
+  <si>
+    <t>Iteration</t>
+  </si>
+  <si>
+    <t>fao_views_key_crop</t>
+  </si>
+  <si>
+    <t>fao_views_year_end</t>
+  </si>
+  <si>
+    <t>year_end</t>
+  </si>
+  <si>
+    <t>Country or Area</t>
+  </si>
+  <si>
+    <t>fao_views_name_country_origin</t>
+  </si>
+  <si>
+    <t>Answer_id</t>
+  </si>
+  <si>
+    <t>StakeHolder</t>
+  </si>
+  <si>
+    <t>Instcode</t>
+  </si>
+  <si>
+    <t>Crop_original</t>
+  </si>
+  <si>
+    <t>SOW2_grouping</t>
+  </si>
+  <si>
+    <t>SOW2_grouping_cleaned</t>
+  </si>
+  <si>
+    <t>PL_group</t>
+  </si>
+  <si>
+    <t>PL_group_cleaned</t>
+  </si>
+  <si>
+    <t>Taxon</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Farmer_varieties</t>
+  </si>
+  <si>
+    <t>Total_Accs</t>
+  </si>
+  <si>
+    <t>Accs_to_NARC</t>
+  </si>
+  <si>
+    <t>Accs_to_PrivateSector</t>
+  </si>
+  <si>
+    <t>Accs_to_FarmerOrNGO</t>
+  </si>
+  <si>
+    <t>Accs_to_Others</t>
+  </si>
+  <si>
+    <t>Accs_to_ForeignStakeholders</t>
+  </si>
+  <si>
+    <t>Accs_to_Unknown</t>
+  </si>
+  <si>
+    <t>Total_Samples</t>
+  </si>
+  <si>
+    <t>Samples_to_NARCs</t>
+  </si>
+  <si>
+    <t>Samples_to_PrivateSector</t>
+  </si>
+  <si>
+    <t>Samples_to_FarmerOrNGO</t>
+  </si>
+  <si>
+    <t>Samples_to_Others</t>
+  </si>
+  <si>
+    <t>Samples_to_ForeignStakeholders</t>
+  </si>
+  <si>
+    <t>Samples_to_Unknown</t>
+  </si>
+  <si>
+    <t>CropList_Common name - main</t>
+  </si>
+  <si>
+    <t>CropList_Common name - alternates</t>
+  </si>
+  <si>
+    <t>CropList_Genera - main</t>
+  </si>
+  <si>
+    <t>CropLIst_Genera - all related</t>
+  </si>
+  <si>
+    <t>CropList_Taxa</t>
+  </si>
+  <si>
+    <t>CropList_Use - primary</t>
+  </si>
+  <si>
+    <t>CropList_Use - detailed</t>
+  </si>
+  <si>
+    <t>CropList_Included in MLS Annex 1</t>
+  </si>
+  <si>
+    <t>CropList_CGIAR mandate</t>
+  </si>
+  <si>
+    <t>Region Code</t>
+  </si>
+  <si>
+    <t>Region Name</t>
+  </si>
+  <si>
+    <t>Sub-region Code</t>
+  </si>
+  <si>
+    <t>Sub-region Name</t>
+  </si>
+  <si>
+    <t>Intermediate Region Code</t>
+  </si>
+  <si>
+    <t>Intermediate Region Name</t>
+  </si>
+  <si>
+    <t>ISO-alpha2 Code</t>
+  </si>
+  <si>
+    <t>Least Developed Countries (LDC)</t>
+  </si>
+  <si>
+    <t>Land Locked Developing Countries (LLDC)</t>
+  </si>
+  <si>
+    <t>Small Island Developing States (SIDS)</t>
+  </si>
+  <si>
+    <t>year_start</t>
+  </si>
+  <si>
+    <t>crop_x</t>
+  </si>
+  <si>
+    <t>Production_x</t>
+  </si>
+  <si>
+    <t>Ratification_1</t>
+  </si>
+  <si>
+    <t>Party_cleaned</t>
+  </si>
+  <si>
+    <t>Contracting Party</t>
+  </si>
+  <si>
+    <t>Contracting Party_cleaned</t>
+  </si>
+  <si>
+    <t>Entry into Force</t>
+  </si>
+  <si>
+    <t>FAO_WIEWS_fulldataset_wcroplistdata_2022_4_6.xlsx</t>
+  </si>
+  <si>
+    <t>iso3_original</t>
+  </si>
+  <si>
+    <t>Nagoya_Country Ratification_02.08.22_cleaned_2022_4_6.xlsx</t>
   </si>
 </sst>
 </file>
@@ -5383,10 +5591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5453,7 +5661,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B8" t="s">
         <v>1454</v>
@@ -5461,7 +5669,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="B9" t="s">
         <v>1460</v>
@@ -5589,10 +5797,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="B25" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -5632,7 +5840,7 @@
         <v>1576</v>
       </c>
       <c r="B30" t="s">
-        <v>1581</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -5653,31 +5861,31 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B33" t="s">
         <v>1602</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1603</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="B34" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="B35" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="B36" t="s">
         <v>1421</v>
@@ -5685,10 +5893,82 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="B37" t="s">
-        <v>1610</v>
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1676</v>
       </c>
     </row>
   </sheetData>
@@ -5702,7 +5982,7 @@
   <dimension ref="A1:BJ356"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39257,8 +39537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C2A8A4-DA1A-428D-90DC-2778CD784C14}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39272,13 +39552,13 @@
         <v>1506</v>
       </c>
       <c r="B1" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="C1" t="s">
         <v>1507</v>
       </c>
       <c r="D1" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="E1" t="s">
         <v>1574</v>
@@ -39343,7 +39623,7 @@
         <v>1451</v>
       </c>
       <c r="C5" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -39462,7 +39742,7 @@
         <v>1511</v>
       </c>
       <c r="C12" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -39564,7 +39844,7 @@
         <v>1534</v>
       </c>
       <c r="C18" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -39632,7 +39912,7 @@
         <v>1537</v>
       </c>
       <c r="C22" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -40459,13 +40739,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="B71" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C71" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -40476,13 +40756,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="B72" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="C72" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -40493,13 +40773,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="B73" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="C73" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -40510,13 +40790,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B74" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C74" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -40530,10 +40810,10 @@
         <v>1451</v>
       </c>
       <c r="B75" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="C75" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -40544,13 +40824,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B76" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="C76" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -40561,13 +40841,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B77" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C77" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -40578,13 +40858,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="B78" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="C78" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -40595,13 +40875,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="B79" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="C79" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -40612,13 +40892,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="B80" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="C80" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -40629,13 +40909,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="B81" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="C81" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -40646,13 +40926,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B82" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="C82" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -40663,13 +40943,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="B83" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="C83" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -40680,13 +40960,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="B84" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="C84" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -40697,13 +40977,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="B85" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="C85" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -40714,13 +40994,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B86" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="C86" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -40731,13 +41011,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="B87" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="C87" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -40748,13 +41028,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="B88" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="C88" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -40765,13 +41045,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B89" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="C89" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -40782,13 +41062,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="B90" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="C90" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -40799,13 +41079,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="B91" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="C91" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -40816,13 +41096,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="B92" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="C92" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -40833,13 +41113,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="B93" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="C93" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -40850,13 +41130,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="B94" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C94" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -40867,13 +41147,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="B95" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="C95" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -40884,13 +41164,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="B96" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="C96" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -40901,13 +41181,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="B97" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="C97" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -40918,13 +41198,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="B98" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="C98" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -40935,13 +41215,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B99" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="C99" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -40952,19 +41232,1793 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B100" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="C100" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="D100">
         <v>1</v>
       </c>
       <c r="E100">
         <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1652</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1640</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1640</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1641</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74B5E72-5BD4-46F0-A381-F91754679733}">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C95" sqref="C95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
+    <col min="5" max="5" width="4.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1653</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1654</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1678</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1679</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1680</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1682</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1682</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1683</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1684</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1684</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1686</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1690</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1691</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1694</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1696</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1698</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1699</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1702</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1703</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1671</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1705</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1706</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1707</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1708</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1708</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1709</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1712</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1732</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1713</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1714</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1715</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1716</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1717</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1718</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1719</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1720</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1721</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1721</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1722</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1723</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1675</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1493</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1499</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1725</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1503</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1504</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1612</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1613</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1614</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1616</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1617</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1618</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1619</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1620</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1620</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1583</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1726</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1727</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1602</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1602</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1599</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1587</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1729</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1730</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1609</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -40972,49 +43026,15 @@
         <v>1640</v>
       </c>
       <c r="B101" t="s">
-        <v>1653</v>
+        <v>1640</v>
       </c>
       <c r="C101" t="s">
-        <v>1653</v>
+        <v>1640</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>1641</v>
-      </c>
-      <c r="B102" t="s">
-        <v>1641</v>
-      </c>
-      <c r="C102" t="s">
-        <v>1641</v>
-      </c>
-      <c r="D102">
-        <v>0</v>
-      </c>
-      <c r="E102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>1642</v>
-      </c>
-      <c r="B103" t="s">
-        <v>1642</v>
-      </c>
-      <c r="C103" t="s">
-        <v>1642</v>
-      </c>
-      <c r="D103">
-        <v>0</v>
-      </c>
-      <c r="E103">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change the years for fao_views with nagoya and treaty data. further the headers was updated
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\fao_sow\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153CD56C-CB3E-4588-A799-C310C9C9794F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE5FB51-1055-4FC9-9324-9C691C5CAF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11651" uniqueCount="1734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11651" uniqueCount="1809">
   <si>
     <t>value</t>
   </si>
@@ -4782,6 +4782,9 @@
     <t>Country</t>
   </si>
   <si>
+    <t>Nagoya_Country Ratification_02.08.22_cleaned.xlsx</t>
+  </si>
+  <si>
     <t>treaty_name_country_origin</t>
   </si>
   <si>
@@ -5238,7 +5241,229 @@
     <t>iso3_original</t>
   </si>
   <si>
-    <t>Nagoya_Country Ratification_02.08.22_cleaned_2022_4_6.xlsx</t>
+    <t>answer_id</t>
+  </si>
+  <si>
+    <t>iteration</t>
+  </si>
+  <si>
+    <t>stakeholder</t>
+  </si>
+  <si>
+    <t>instcode</t>
+  </si>
+  <si>
+    <t>sow2_grouping</t>
+  </si>
+  <si>
+    <t>sow2_grouping_cleaned</t>
+  </si>
+  <si>
+    <t>pl_group</t>
+  </si>
+  <si>
+    <t>pl_group_cleaned</t>
+  </si>
+  <si>
+    <t>taxon</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>farmer_varieties</t>
+  </si>
+  <si>
+    <t>total_accs</t>
+  </si>
+  <si>
+    <t>accs_to_narc</t>
+  </si>
+  <si>
+    <t>accs_to_privatesector</t>
+  </si>
+  <si>
+    <t>accs_to_farmerorngo</t>
+  </si>
+  <si>
+    <t>accs_to_others</t>
+  </si>
+  <si>
+    <t>accs_to_foreignstakeholders</t>
+  </si>
+  <si>
+    <t>accs_to_unknown</t>
+  </si>
+  <si>
+    <t>total_samples</t>
+  </si>
+  <si>
+    <t>samples_to_narcs</t>
+  </si>
+  <si>
+    <t>samples_to_privatesector</t>
+  </si>
+  <si>
+    <t>samples_to_farmerorngo</t>
+  </si>
+  <si>
+    <t>samples_to_others</t>
+  </si>
+  <si>
+    <t>samples_to_foreignstakeholders</t>
+  </si>
+  <si>
+    <t>samples_to_unknown</t>
+  </si>
+  <si>
+    <t>croplist_equivalent</t>
+  </si>
+  <si>
+    <t>croplist_common_name_-_main</t>
+  </si>
+  <si>
+    <t>croplist_common_name_-_alternates</t>
+  </si>
+  <si>
+    <t>croplist_genera_-_main</t>
+  </si>
+  <si>
+    <t>croplist_genera_-_all_related</t>
+  </si>
+  <si>
+    <t>croplist_taxa</t>
+  </si>
+  <si>
+    <t>croplist_use_-_primary</t>
+  </si>
+  <si>
+    <t>croplist_use_-_detailed</t>
+  </si>
+  <si>
+    <t>croplist_included_in_mls_annex_1</t>
+  </si>
+  <si>
+    <t>croplist_cgiar_mandate</t>
+  </si>
+  <si>
+    <t>croplist_seed_storage_behaviour</t>
+  </si>
+  <si>
+    <t>region_code</t>
+  </si>
+  <si>
+    <t>region_name</t>
+  </si>
+  <si>
+    <t>sub-region_code</t>
+  </si>
+  <si>
+    <t>sub-region_name</t>
+  </si>
+  <si>
+    <t>intermediate_region_code</t>
+  </si>
+  <si>
+    <t>intermediate_region_name</t>
+  </si>
+  <si>
+    <t>country_or_area</t>
+  </si>
+  <si>
+    <t>iso-alpha2_code</t>
+  </si>
+  <si>
+    <t>iso-alpha3_code</t>
+  </si>
+  <si>
+    <t>least_developed_countries_(ldc)</t>
+  </si>
+  <si>
+    <t>land_locked_developing_countries_(lldc)</t>
+  </si>
+  <si>
+    <t>small_island_developing_states_(sids)</t>
+  </si>
+  <si>
+    <t>income_level</t>
+  </si>
+  <si>
+    <t>fat_supply_quantity_(g/capita/day)</t>
+  </si>
+  <si>
+    <t>food_supply_(kcal/capita/day)</t>
+  </si>
+  <si>
+    <t>food_supply_quantity_(kg/capita/yr)</t>
+  </si>
+  <si>
+    <t>other_uses_(non-food)</t>
+  </si>
+  <si>
+    <t>production_x</t>
+  </si>
+  <si>
+    <t>protein_supply_quantity_(g/capita/day)</t>
+  </si>
+  <si>
+    <t>area_harvested</t>
+  </si>
+  <si>
+    <t>production_y</t>
+  </si>
+  <si>
+    <t>yield</t>
+  </si>
+  <si>
+    <t>gross_production_value_(constant_2014-2016_thousand_i$)</t>
+  </si>
+  <si>
+    <t>gross_production_value_(constant_2014-2016_thousand_slc)</t>
+  </si>
+  <si>
+    <t>gross_production_value_(constant_2014-2016_thousand_us$)</t>
+  </si>
+  <si>
+    <t>gross_production_value_(current_thousand_slc)</t>
+  </si>
+  <si>
+    <t>gross_production_value_(current_thousand_us$)</t>
+  </si>
+  <si>
+    <t>country_x</t>
+  </si>
+  <si>
+    <t>nagoya_ratification_1</t>
+  </si>
+  <si>
+    <t>nagoya_party_cleaned</t>
+  </si>
+  <si>
+    <t>nagoya_party_year_cleaned</t>
+  </si>
+  <si>
+    <t>distributor_signatory_nagoya_transfer</t>
+  </si>
+  <si>
+    <t>country_y</t>
+  </si>
+  <si>
+    <t>contracting_party</t>
+  </si>
+  <si>
+    <t>planttreaty_contracting_party_cleaned</t>
+  </si>
+  <si>
+    <t>entry_into_force</t>
+  </si>
+  <si>
+    <t>planttreaty_entry_into_force_cleaned</t>
+  </si>
+  <si>
+    <t>origin_member_planttreaty_transfer</t>
   </si>
 </sst>
 </file>
@@ -5593,8 +5818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5661,7 +5886,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="B8" t="s">
         <v>1454</v>
@@ -5669,7 +5894,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="B9" t="s">
         <v>1460</v>
@@ -5797,10 +6022,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B25" t="s">
         <v>1611</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1610</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -5840,7 +6065,7 @@
         <v>1576</v>
       </c>
       <c r="B30" t="s">
-        <v>1733</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -5861,31 +6086,31 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="B33" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="B34" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="B35" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="B36" t="s">
         <v>1421</v>
@@ -5893,15 +6118,15 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="B37" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
@@ -5909,31 +6134,31 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="B39" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="B40" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="B41" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="B42" t="s">
         <v>1432</v>
@@ -5941,7 +6166,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="B43" t="s">
         <v>1442</v>
@@ -5949,26 +6174,26 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="B44" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="B45" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B46" t="s">
         <v>1677</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1676</v>
       </c>
     </row>
   </sheetData>
@@ -39537,14 +39762,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C2A8A4-DA1A-428D-90DC-2778CD784C14}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -39552,13 +39778,13 @@
         <v>1506</v>
       </c>
       <c r="B1" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="C1" t="s">
         <v>1507</v>
       </c>
       <c r="D1" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="E1" t="s">
         <v>1574</v>
@@ -39623,7 +39849,7 @@
         <v>1451</v>
       </c>
       <c r="C5" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -39742,7 +39968,7 @@
         <v>1511</v>
       </c>
       <c r="C12" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -39844,7 +40070,7 @@
         <v>1534</v>
       </c>
       <c r="C18" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -39912,7 +40138,7 @@
         <v>1537</v>
       </c>
       <c r="C22" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -40739,13 +40965,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="B71" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="C71" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -40756,13 +40982,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="B72" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="C72" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -40773,13 +40999,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="B73" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="C73" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -40790,13 +41016,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="B74" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="C74" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -40810,10 +41036,10 @@
         <v>1451</v>
       </c>
       <c r="B75" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="C75" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -40824,13 +41050,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="B76" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="C76" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -40841,13 +41067,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="B77" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="C77" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -40858,13 +41084,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="B78" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="C78" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -40875,13 +41101,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="B79" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="C79" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -40892,13 +41118,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="B80" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="C80" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -40909,13 +41135,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="B81" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="C81" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -40926,13 +41152,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="B82" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="C82" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -40943,13 +41169,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="B83" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="C83" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -40960,13 +41186,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="B84" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="C84" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -40977,13 +41203,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="B85" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="C85" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -40994,13 +41220,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="B86" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="C86" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -41011,13 +41237,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="B87" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="C87" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -41028,13 +41254,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="B88" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="C88" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -41045,13 +41271,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="B89" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="C89" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -41062,13 +41288,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="B90" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="C90" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -41079,13 +41305,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="B91" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="C91" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -41096,13 +41322,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="B92" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="C92" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -41113,13 +41339,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="B93" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="C93" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -41130,13 +41356,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="B94" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="C94" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -41147,13 +41373,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="B95" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="C95" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -41164,13 +41390,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="B96" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="C96" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -41181,13 +41407,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="B97" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="C97" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -41198,13 +41424,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="B98" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="C98" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -41215,13 +41441,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="B99" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="C99" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -41232,13 +41458,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="B100" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="C100" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -41249,13 +41475,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="B101" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="C101" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -41266,13 +41492,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="B102" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="C102" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -41283,13 +41509,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="B103" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="C103" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -41307,16 +41533,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74B5E72-5BD4-46F0-A381-F91754679733}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C95" sqref="C95"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.21875" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.21875" customWidth="1"/>
     <col min="5" max="5" width="4.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -41326,13 +41554,13 @@
         <v>1506</v>
       </c>
       <c r="B1" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="C1" t="s">
         <v>1507</v>
       </c>
       <c r="D1" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="E1" t="s">
         <v>1574</v>
@@ -41357,13 +41585,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="B3" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="C3" t="s">
-        <v>1678</v>
+        <v>1734</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -41374,13 +41602,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="B4" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="C4" t="s">
-        <v>1672</v>
+        <v>1735</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -41408,13 +41636,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="B6" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="C6" t="s">
-        <v>1679</v>
+        <v>1736</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -41425,13 +41653,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="B7" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="C7" t="s">
-        <v>1680</v>
+        <v>1737</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -41442,13 +41670,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="B8" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="C8" t="s">
-        <v>1681</v>
+        <v>1656</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -41465,7 +41693,7 @@
         <v>1442</v>
       </c>
       <c r="C9" t="s">
-        <v>1442</v>
+        <v>1509</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -41476,13 +41704,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="B10" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="C10" t="s">
-        <v>1682</v>
+        <v>1738</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -41493,13 +41721,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="B11" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="C11" t="s">
-        <v>1683</v>
+        <v>1739</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -41510,13 +41738,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="B12" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="C12" t="s">
-        <v>1684</v>
+        <v>1740</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -41527,13 +41755,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="B13" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="C13" t="s">
-        <v>1685</v>
+        <v>1741</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -41544,13 +41772,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="B14" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="C14" t="s">
-        <v>1686</v>
+        <v>1742</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -41561,13 +41789,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="B15" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="C15" t="s">
-        <v>1687</v>
+        <v>1743</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -41578,13 +41806,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B16" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="C16" t="s">
-        <v>1688</v>
+        <v>1744</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -41612,13 +41840,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="B18" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="C18" t="s">
-        <v>1689</v>
+        <v>1745</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -41629,13 +41857,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="B19" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="C19" t="s">
-        <v>1690</v>
+        <v>1746</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -41646,13 +41874,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="B20" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="C20" t="s">
-        <v>1691</v>
+        <v>1747</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -41663,13 +41891,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="B21" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="C21" t="s">
-        <v>1692</v>
+        <v>1748</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -41680,13 +41908,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="B22" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="C22" t="s">
-        <v>1693</v>
+        <v>1749</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -41697,13 +41925,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="B23" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="C23" t="s">
-        <v>1694</v>
+        <v>1750</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -41714,13 +41942,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="B24" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="C24" t="s">
-        <v>1695</v>
+        <v>1751</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -41731,13 +41959,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="B25" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="C25" t="s">
-        <v>1696</v>
+        <v>1752</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -41748,13 +41976,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="B26" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="C26" t="s">
-        <v>1697</v>
+        <v>1753</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -41765,13 +41993,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="B27" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="C27" t="s">
-        <v>1698</v>
+        <v>1754</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -41782,13 +42010,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="B28" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="C28" t="s">
-        <v>1699</v>
+        <v>1755</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -41799,13 +42027,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="B29" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="C29" t="s">
-        <v>1700</v>
+        <v>1756</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -41816,13 +42044,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="B30" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="C30" t="s">
-        <v>1701</v>
+        <v>1757</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -41833,13 +42061,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="B31" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="C31" t="s">
-        <v>1702</v>
+        <v>1758</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -41850,13 +42078,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="B32" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="C32" t="s">
-        <v>1703</v>
+        <v>1759</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -41867,13 +42095,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="B33" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="C33" t="s">
-        <v>1671</v>
+        <v>1760</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -41884,13 +42112,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="B34" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="C34" t="s">
-        <v>1704</v>
+        <v>1761</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -41901,13 +42129,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="B35" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="C35" t="s">
-        <v>1705</v>
+        <v>1762</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -41918,13 +42146,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="B36" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="C36" t="s">
-        <v>1706</v>
+        <v>1763</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -41935,13 +42163,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="B37" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="C37" t="s">
-        <v>1707</v>
+        <v>1764</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -41952,13 +42180,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="B38" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="C38" t="s">
-        <v>1708</v>
+        <v>1765</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -41969,13 +42197,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="B39" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="C39" t="s">
-        <v>1709</v>
+        <v>1766</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -41986,13 +42214,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="B40" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="C40" t="s">
-        <v>1710</v>
+        <v>1767</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -42003,13 +42231,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="B41" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="C41" t="s">
-        <v>1711</v>
+        <v>1768</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -42020,13 +42248,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="B42" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="C42" t="s">
-        <v>1712</v>
+        <v>1769</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -42043,7 +42271,7 @@
         <v>1110</v>
       </c>
       <c r="C43" t="s">
-        <v>1110</v>
+        <v>1770</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -42054,13 +42282,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="B44" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="C44" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -42071,13 +42299,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="B45" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="C45" t="s">
-        <v>1713</v>
+        <v>1771</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -42088,13 +42316,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="B46" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="C46" t="s">
-        <v>1714</v>
+        <v>1772</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -42105,13 +42333,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="B47" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="C47" t="s">
-        <v>1715</v>
+        <v>1773</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -42122,13 +42350,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="B48" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="C48" t="s">
-        <v>1716</v>
+        <v>1774</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -42139,13 +42367,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="B49" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="C49" t="s">
-        <v>1717</v>
+        <v>1775</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -42156,13 +42384,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="B50" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="C50" t="s">
-        <v>1718</v>
+        <v>1776</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -42173,13 +42401,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="B51" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="C51" t="s">
-        <v>1676</v>
+        <v>1777</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -42190,13 +42418,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="B52" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="C52" t="s">
-        <v>1719</v>
+        <v>1778</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -42213,7 +42441,7 @@
         <v>1417</v>
       </c>
       <c r="C53" t="s">
-        <v>1417</v>
+        <v>1779</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -42224,13 +42452,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="B54" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="C54" t="s">
-        <v>1720</v>
+        <v>1780</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -42241,13 +42469,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="B55" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="C55" t="s">
-        <v>1721</v>
+        <v>1781</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -42258,13 +42486,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="B56" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="C56" t="s">
-        <v>1722</v>
+        <v>1782</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -42275,13 +42503,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="B57" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="C57" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -42292,13 +42520,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="B58" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="C58" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -42332,7 +42560,7 @@
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>0</v>
+        <v>1783</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -42349,7 +42577,7 @@
         <v>1489</v>
       </c>
       <c r="C61" t="s">
-        <v>1489</v>
+        <v>1538</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -42360,13 +42588,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="B62" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="C62" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -42383,7 +42611,7 @@
         <v>1490</v>
       </c>
       <c r="C63" t="s">
-        <v>1490</v>
+        <v>1539</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -42400,7 +42628,7 @@
         <v>1491</v>
       </c>
       <c r="C64" t="s">
-        <v>1491</v>
+        <v>1568</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -42417,7 +42645,7 @@
         <v>1492</v>
       </c>
       <c r="C65" t="s">
-        <v>1492</v>
+        <v>1784</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -42434,7 +42662,7 @@
         <v>1493</v>
       </c>
       <c r="C66" t="s">
-        <v>1493</v>
+        <v>1526</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -42451,7 +42679,7 @@
         <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>22</v>
+        <v>1527</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -42468,7 +42696,7 @@
         <v>1494</v>
       </c>
       <c r="C68" t="s">
-        <v>1494</v>
+        <v>1785</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -42485,7 +42713,7 @@
         <v>1495</v>
       </c>
       <c r="C69" t="s">
-        <v>1495</v>
+        <v>1786</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -42502,7 +42730,7 @@
         <v>1496</v>
       </c>
       <c r="C70" t="s">
-        <v>1496</v>
+        <v>1572</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -42519,7 +42747,7 @@
         <v>1497</v>
       </c>
       <c r="C71" t="s">
-        <v>1497</v>
+        <v>1528</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -42536,7 +42764,7 @@
         <v>1498</v>
       </c>
       <c r="C72" t="s">
-        <v>1498</v>
+        <v>1787</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -42553,7 +42781,7 @@
         <v>1499</v>
       </c>
       <c r="C73" t="s">
-        <v>1499</v>
+        <v>1529</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -42564,13 +42792,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="B74" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="C74" t="s">
-        <v>1725</v>
+        <v>1788</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -42587,7 +42815,7 @@
         <v>1501</v>
       </c>
       <c r="C75" t="s">
-        <v>1501</v>
+        <v>1789</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -42604,7 +42832,7 @@
         <v>1502</v>
       </c>
       <c r="C76" t="s">
-        <v>1502</v>
+        <v>1531</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -42621,7 +42849,7 @@
         <v>1503</v>
       </c>
       <c r="C77" t="s">
-        <v>1503</v>
+        <v>1532</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -42638,7 +42866,7 @@
         <v>1504</v>
       </c>
       <c r="C78" t="s">
-        <v>1504</v>
+        <v>1573</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -42655,7 +42883,7 @@
         <v>1505</v>
       </c>
       <c r="C79" t="s">
-        <v>1505</v>
+        <v>1533</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -42666,13 +42894,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="B80" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="C80" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -42683,13 +42911,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="B81" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="C81" t="s">
-        <v>1613</v>
+        <v>1790</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -42700,13 +42928,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="B82" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="C82" t="s">
-        <v>1614</v>
+        <v>1791</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -42717,13 +42945,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="B83" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="C83" t="s">
-        <v>1615</v>
+        <v>1792</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -42751,13 +42979,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="B85" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="C85" t="s">
-        <v>1616</v>
+        <v>1793</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -42768,13 +42996,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="B86" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="C86" t="s">
-        <v>1617</v>
+        <v>1794</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -42785,13 +43013,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="B87" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="C87" t="s">
-        <v>1618</v>
+        <v>1795</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -42802,13 +43030,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="B88" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="C88" t="s">
-        <v>1619</v>
+        <v>1796</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -42819,13 +43047,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="B89" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="C89" t="s">
-        <v>1620</v>
+        <v>1797</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -42836,13 +43064,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="B90" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="C90" t="s">
-        <v>1583</v>
+        <v>1798</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -42853,13 +43081,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="B91" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="C91" t="s">
-        <v>1726</v>
+        <v>1799</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -42870,13 +43098,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="B92" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="C92" t="s">
-        <v>1727</v>
+        <v>1800</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -42887,13 +43115,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="B93" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="C93" t="s">
-        <v>1602</v>
+        <v>1801</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -42904,13 +43132,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="B94" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="C94" t="s">
-        <v>1599</v>
+        <v>1802</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -42921,13 +43149,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="B95" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="C95" t="s">
-        <v>1587</v>
+        <v>1803</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -42944,7 +43172,7 @@
         <v>1421</v>
       </c>
       <c r="C96" t="s">
-        <v>1421</v>
+        <v>1432</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -42955,13 +43183,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="B97" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="C97" t="s">
-        <v>1728</v>
+        <v>1804</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -42972,13 +43200,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="B98" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="C98" t="s">
-        <v>1729</v>
+        <v>1805</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -42989,13 +43217,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="B99" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="C99" t="s">
-        <v>1730</v>
+        <v>1806</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -43006,13 +43234,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="B100" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="C100" t="s">
-        <v>1609</v>
+        <v>1807</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -43023,13 +43251,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="B101" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="C101" t="s">
-        <v>1640</v>
+        <v>1808</v>
       </c>
       <c r="D101">
         <v>0</v>

</xml_diff>

<commit_message>
fixed some bugs with names in configuration files
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\fao_sow\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD96AED1-E3C0-41DB-89C4-35648FD0D65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCF6419-07D8-4C80-850D-3FB130B6EF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -5661,8 +5661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40783,7 +40783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74B5E72-5BD4-46F0-A381-F91754679733}">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>